<commit_message>
code impoved a little
</commit_message>
<xml_diff>
--- a/texts/id_12 gisele.xlsx
+++ b/texts/id_12 gisele.xlsx
@@ -7,7 +7,8 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="01.06.-31.08." sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="01.09-30.09" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="01.10-31.10" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>Общие метрики</t>
   </si>
@@ -71,7 +72,7 @@
     <t>Клики по автоподказкам</t>
   </si>
   <si>
-    <t>1295</t>
+    <t>0350</t>
   </si>
   <si>
     <t>Выручка, руб.</t>
@@ -83,70 +84,127 @@
     <t>Товары</t>
   </si>
   <si>
+    <t>1 0109</t>
+  </si>
+  <si>
+    <t>Категории</t>
+  </si>
+  <si>
+    <t>арт 1 0113</t>
+  </si>
+  <si>
+    <t>Запросы</t>
+  </si>
+  <si>
+    <t>чулки</t>
+  </si>
+  <si>
+    <t>0130</t>
+  </si>
+  <si>
+    <t>1 0320</t>
+  </si>
+  <si>
+    <t>Исправления</t>
+  </si>
+  <si>
+    <t>1 0350 black</t>
+  </si>
+  <si>
+    <t>1 0353</t>
+  </si>
+  <si>
+    <t>30130</t>
+  </si>
+  <si>
+    <t>33098</t>
+  </si>
+  <si>
+    <t>dita von</t>
+  </si>
+  <si>
+    <t>kjok</t>
+  </si>
+  <si>
+    <t>lounge</t>
+  </si>
+  <si>
+    <t>rosapois</t>
+  </si>
+  <si>
+    <t>valery</t>
+  </si>
+  <si>
+    <t>платья</t>
+  </si>
+  <si>
+    <t>пояс</t>
+  </si>
+  <si>
+    <t>просто</t>
+  </si>
+  <si>
+    <t>слитные купальники</t>
+  </si>
+  <si>
+    <t>туники</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>комплект</t>
+  </si>
+  <si>
+    <t>трусы</t>
+  </si>
+  <si>
+    <t>1970</t>
+  </si>
+  <si>
+    <t>2 0343</t>
+  </si>
+  <si>
+    <t>2 0344g</t>
+  </si>
+  <si>
+    <t>3559</t>
+  </si>
+  <si>
+    <t>452</t>
+  </si>
+  <si>
+    <t>65982</t>
+  </si>
+  <si>
+    <t>capacidad</t>
+  </si>
+  <si>
+    <t>la perla</t>
+  </si>
+  <si>
     <t>lafabbricadellino</t>
   </si>
   <si>
-    <t>Категории</t>
-  </si>
-  <si>
-    <t>стринги</t>
-  </si>
-  <si>
-    <t>Запросы</t>
-  </si>
-  <si>
-    <t>трусы</t>
-  </si>
-  <si>
-    <t>0263</t>
-  </si>
-  <si>
-    <t>lounge</t>
-  </si>
-  <si>
-    <t>Исправления</t>
-  </si>
-  <si>
-    <t>купальник</t>
-  </si>
-  <si>
-    <t>купальник раздельный 3 3126</t>
-  </si>
-  <si>
-    <t>куртка</t>
-  </si>
-  <si>
-    <t>рапр</t>
-  </si>
-  <si>
-    <t>синий</t>
-  </si>
-  <si>
-    <t>тыва</t>
-  </si>
-  <si>
-    <t>1 0357</t>
-  </si>
-  <si>
-    <t>3280</t>
-  </si>
-  <si>
-    <t>lou paris</t>
-  </si>
-  <si>
-    <t>nessa valerie</t>
-  </si>
-  <si>
-    <t>боди</t>
-  </si>
-  <si>
-    <t>прозрачная спина</t>
+    <t>parah</t>
+  </si>
+  <si>
+    <t>женская одежда 50 размера</t>
+  </si>
+  <si>
+    <t>купальник раздельный</t>
+  </si>
+  <si>
+    <t>купол</t>
+  </si>
+  <si>
+    <t>носки</t>
+  </si>
+  <si>
+    <t>пеньюар</t>
   </si>
   <si>
     <t>топ</t>
-  </si>
-  <si>
-    <t>уверены</t>
   </si>
 </sst>
 </file>
@@ -164,11 +222,11 @@
     </font>
     <font>
       <name val="Arial"/>
+      <b val="1"/>
       <sz val="11"/>
     </font>
     <font>
       <name val="Arial"/>
-      <b val="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -196,31 +254,31 @@
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="3">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="3">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -539,7 +597,7 @@
     <col customWidth="1" max="6" min="6" width="15"/>
     <col customWidth="1" max="7" min="7" width="15"/>
     <col customWidth="1" max="8" min="8" width="15"/>
-    <col customWidth="1" max="9" min="9" width="29.7"/>
+    <col customWidth="1" max="9" min="9" width="19.8"/>
     <col customWidth="1" max="10" min="10" width="15"/>
     <col customWidth="1" max="11" min="11" width="15"/>
     <col customWidth="1" max="12" min="12" width="15"/>
@@ -581,7 +639,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n"/>
@@ -591,29 +649,29 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>6226</v>
+        <v>1997</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>282195</v>
+        <v>26548</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>0.0024092515258593</v>
+        <v>0</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>45.33</v>
+        <v>13.29</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>18813</v>
+        <v>13274</v>
       </c>
       <c r="H3" s="2" t="n"/>
       <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="K3" s="2" t="n"/>
       <c r="L3" s="2" t="n"/>
@@ -623,22 +681,22 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>6168</v>
+        <v>1975</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>265697</v>
+        <v>26548</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0.002107652399481193</v>
+        <v>0</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>43.08</v>
+        <v>13.44</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>20438.23</v>
+        <v>13274</v>
       </c>
       <c r="H4" s="2" t="n"/>
       <c r="I4" s="2" t="n"/>
@@ -651,22 +709,22 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>16498</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.03448275862068965</v>
+        <v>0</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>284.45</v>
+        <v>0</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>8249</v>
+        <v>0</v>
       </c>
       <c r="H5" s="2" t="n"/>
       <c r="I5" s="2" t="n"/>
@@ -679,13 +737,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>0.009315772566655958</v>
+        <v>0.01</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>0.1333333333333333</v>
+        <v>0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>0.05846311947412251</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2" t="n"/>
       <c r="F6" s="2" t="n"/>
@@ -741,7 +799,7 @@
         <v>18</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K9" s="2" t="n"/>
       <c r="L9" s="2" t="n"/>
@@ -773,14 +831,14 @@
         <v>22</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K10" s="2" t="n"/>
       <c r="L10" s="2" t="n"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>0</v>
@@ -789,7 +847,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="7" t="n">
-        <v>0.06900000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E11" s="7" t="n">
         <v>0</v>
@@ -805,7 +863,7 @@
         <v>24</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K11" s="2" t="n"/>
       <c r="L11" s="2" t="n"/>
@@ -820,14 +878,14 @@
         <v>25</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2" t="n"/>
       <c r="I12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K12" s="2" t="n"/>
       <c r="L12" s="2" t="n"/>
@@ -842,14 +900,14 @@
         <v>9</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H13" s="2" t="n"/>
       <c r="I13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K13" s="2" t="n"/>
       <c r="L13" s="2" t="n"/>
@@ -867,7 +925,7 @@
         <v>28</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14" s="2" t="n"/>
       <c r="L14" s="2" t="n"/>
@@ -885,7 +943,7 @@
         <v>30</v>
       </c>
       <c r="J15" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K15" s="2" t="n"/>
       <c r="L15" s="2" t="n"/>
@@ -909,20 +967,20 @@
         <v>31</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" s="2" t="n"/>
       <c r="L16" s="2" t="n"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="6" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B17" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>9699</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="n"/>
       <c r="E17" s="2" t="n"/>
@@ -933,7 +991,7 @@
         <v>32</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K17" s="2" t="n"/>
       <c r="L17" s="2" t="n"/>
@@ -951,7 +1009,7 @@
         <v>33</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K18" s="2" t="n"/>
       <c r="L18" s="2" t="n"/>
@@ -969,7 +1027,7 @@
         <v>34</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K19" s="2" t="n"/>
       <c r="L19" s="2" t="n"/>
@@ -987,7 +1045,7 @@
         <v>35</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2" t="n"/>
       <c r="L20" s="2" t="n"/>
@@ -1455,4 +1513,944 @@
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="25"/>
+    <col customWidth="1" max="2" min="2" width="15"/>
+    <col customWidth="1" max="3" min="3" width="15"/>
+    <col customWidth="1" max="4" min="4" width="15"/>
+    <col customWidth="1" max="5" min="5" width="15"/>
+    <col customWidth="1" max="6" min="6" width="15"/>
+    <col customWidth="1" max="7" min="7" width="15"/>
+    <col customWidth="1" max="8" min="8" width="15"/>
+    <col customWidth="1" max="9" min="9" width="27.5"/>
+    <col customWidth="1" max="10" min="10" width="15"/>
+    <col customWidth="1" max="11" min="11" width="15"/>
+    <col customWidth="1" max="12" min="12" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3" t="s"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>2230</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>23338</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>7779.33</v>
+      </c>
+      <c r="H3" s="2" t="n"/>
+      <c r="I3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>2204</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>23338</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>10.59</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>7779.33</v>
+      </c>
+      <c r="H4" s="2" t="n"/>
+      <c r="I4" s="2" t="n"/>
+      <c r="J4" s="2" t="n"/>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n"/>
+      <c r="I5" s="2" t="n"/>
+      <c r="J5" s="2" t="n"/>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" s="2" t="n"/>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="2" t="n"/>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2" t="n"/>
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="2" t="n"/>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="2" t="n"/>
+      <c r="L7" s="2" t="n"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2" t="n"/>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="2" t="n"/>
+      <c r="L8" s="2" t="n"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="2" t="n"/>
+      <c r="I9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2" t="n"/>
+      <c r="L9" s="2" t="n"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="n"/>
+      <c r="I10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="2" t="n"/>
+      <c r="L10" s="2" t="n"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>0.1143</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2" t="n"/>
+      <c r="I11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2" t="n"/>
+      <c r="L11" s="2" t="n"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="2" t="n"/>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="n"/>
+      <c r="I12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2" t="n"/>
+      <c r="L12" s="2" t="n"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="2" t="n"/>
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H13" s="2" t="n"/>
+      <c r="I13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="n"/>
+      <c r="L13" s="2" t="n"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2" t="n"/>
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" s="2" t="n"/>
+      <c r="G14" s="2" t="n"/>
+      <c r="H14" s="2" t="n"/>
+      <c r="I14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="n"/>
+      <c r="L14" s="2" t="n"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="n"/>
+      <c r="H15" s="2" t="n"/>
+      <c r="I15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2" t="n"/>
+      <c r="L15" s="2" t="n"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="n"/>
+      <c r="E16" s="2" t="n"/>
+      <c r="F16" s="2" t="n"/>
+      <c r="G16" s="2" t="n"/>
+      <c r="H16" s="2" t="n"/>
+      <c r="I16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="n"/>
+      <c r="L16" s="2" t="n"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
+      <c r="F17" s="2" t="n"/>
+      <c r="G17" s="2" t="n"/>
+      <c r="H17" s="2" t="n"/>
+      <c r="I17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2" t="n"/>
+      <c r="L17" s="2" t="n"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="2" t="n"/>
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n"/>
+      <c r="E18" s="2" t="n"/>
+      <c r="F18" s="2" t="n"/>
+      <c r="G18" s="2" t="n"/>
+      <c r="H18" s="2" t="n"/>
+      <c r="I18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="n"/>
+      <c r="L18" s="2" t="n"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="2" t="n"/>
+      <c r="B19" s="2" t="n"/>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n"/>
+      <c r="E19" s="2" t="n"/>
+      <c r="F19" s="2" t="n"/>
+      <c r="G19" s="2" t="n"/>
+      <c r="H19" s="2" t="n"/>
+      <c r="I19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="n"/>
+      <c r="L19" s="2" t="n"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="2" t="n"/>
+      <c r="B20" s="2" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
+      <c r="F20" s="2" t="n"/>
+      <c r="G20" s="2" t="n"/>
+      <c r="H20" s="2" t="n"/>
+      <c r="I20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2" t="n"/>
+      <c r="L20" s="2" t="n"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="2" t="n"/>
+      <c r="B21" s="2" t="n"/>
+      <c r="C21" s="2" t="n"/>
+      <c r="D21" s="2" t="n"/>
+      <c r="E21" s="2" t="n"/>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="2" t="n"/>
+      <c r="H21" s="2" t="n"/>
+      <c r="I21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2" t="n"/>
+      <c r="L21" s="2" t="n"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="2" t="n"/>
+      <c r="B22" s="2" t="n"/>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n"/>
+      <c r="E22" s="2" t="n"/>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="2" t="n"/>
+      <c r="H22" s="2" t="n"/>
+      <c r="I22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2" t="n"/>
+      <c r="L22" s="2" t="n"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="2" t="n"/>
+      <c r="B23" s="2" t="n"/>
+      <c r="C23" s="2" t="n"/>
+      <c r="D23" s="2" t="n"/>
+      <c r="E23" s="2" t="n"/>
+      <c r="F23" s="2" t="n"/>
+      <c r="G23" s="2" t="n"/>
+      <c r="H23" s="2" t="n"/>
+      <c r="I23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2" t="n"/>
+      <c r="L23" s="2" t="n"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="2" t="n"/>
+      <c r="B24" s="2" t="n"/>
+      <c r="C24" s="2" t="n"/>
+      <c r="D24" s="2" t="n"/>
+      <c r="E24" s="2" t="n"/>
+      <c r="F24" s="2" t="n"/>
+      <c r="G24" s="2" t="n"/>
+      <c r="H24" s="2" t="n"/>
+      <c r="I24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2" t="n"/>
+      <c r="L24" s="2" t="n"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="2" t="n"/>
+      <c r="B25" s="2" t="n"/>
+      <c r="C25" s="2" t="n"/>
+      <c r="D25" s="2" t="n"/>
+      <c r="E25" s="2" t="n"/>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="2" t="n"/>
+      <c r="H25" s="2" t="n"/>
+      <c r="I25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2" t="n"/>
+      <c r="L25" s="2" t="n"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="2" t="n"/>
+      <c r="B26" s="2" t="n"/>
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="n"/>
+      <c r="E26" s="2" t="n"/>
+      <c r="F26" s="2" t="n"/>
+      <c r="G26" s="2" t="n"/>
+      <c r="H26" s="2" t="n"/>
+      <c r="I26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2" t="n"/>
+      <c r="L26" s="2" t="n"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="2" t="n"/>
+      <c r="B27" s="2" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n"/>
+      <c r="E27" s="2" t="n"/>
+      <c r="F27" s="2" t="n"/>
+      <c r="G27" s="2" t="n"/>
+      <c r="H27" s="2" t="n"/>
+      <c r="I27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2" t="n"/>
+      <c r="L27" s="2" t="n"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="2" t="n"/>
+      <c r="B28" s="2" t="n"/>
+      <c r="C28" s="2" t="n"/>
+      <c r="D28" s="2" t="n"/>
+      <c r="E28" s="2" t="n"/>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="2" t="n"/>
+      <c r="H28" s="2" t="n"/>
+      <c r="I28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" s="2" t="n"/>
+      <c r="L28" s="2" t="n"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="2" t="n"/>
+      <c r="B29" s="2" t="n"/>
+      <c r="C29" s="2" t="n"/>
+      <c r="D29" s="2" t="n"/>
+      <c r="E29" s="2" t="n"/>
+      <c r="F29" s="2" t="n"/>
+      <c r="G29" s="2" t="n"/>
+      <c r="H29" s="2" t="n"/>
+      <c r="I29" s="2" t="n"/>
+      <c r="J29" s="2" t="n"/>
+      <c r="K29" s="2" t="n"/>
+      <c r="L29" s="2" t="n"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2" t="n"/>
+      <c r="B30" s="2" t="n"/>
+      <c r="C30" s="2" t="n"/>
+      <c r="D30" s="2" t="n"/>
+      <c r="E30" s="2" t="n"/>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="2" t="n"/>
+      <c r="H30" s="2" t="n"/>
+      <c r="I30" s="2" t="n"/>
+      <c r="J30" s="2" t="n"/>
+      <c r="K30" s="2" t="n"/>
+      <c r="L30" s="2" t="n"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="2" t="n"/>
+      <c r="B31" s="2" t="n"/>
+      <c r="C31" s="2" t="n"/>
+      <c r="D31" s="2" t="n"/>
+      <c r="E31" s="2" t="n"/>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="2" t="n"/>
+      <c r="H31" s="2" t="n"/>
+      <c r="I31" s="2" t="n"/>
+      <c r="J31" s="2" t="n"/>
+      <c r="K31" s="2" t="n"/>
+      <c r="L31" s="2" t="n"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="2" t="n"/>
+      <c r="B32" s="2" t="n"/>
+      <c r="C32" s="2" t="n"/>
+      <c r="D32" s="2" t="n"/>
+      <c r="E32" s="2" t="n"/>
+      <c r="F32" s="2" t="n"/>
+      <c r="G32" s="2" t="n"/>
+      <c r="H32" s="2" t="n"/>
+      <c r="I32" s="2" t="n"/>
+      <c r="J32" s="2" t="n"/>
+      <c r="K32" s="2" t="n"/>
+      <c r="L32" s="2" t="n"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="2" t="n"/>
+      <c r="B33" s="2" t="n"/>
+      <c r="C33" s="2" t="n"/>
+      <c r="D33" s="2" t="n"/>
+      <c r="E33" s="2" t="n"/>
+      <c r="F33" s="2" t="n"/>
+      <c r="G33" s="2" t="n"/>
+      <c r="H33" s="2" t="n"/>
+      <c r="I33" s="2" t="n"/>
+      <c r="J33" s="2" t="n"/>
+      <c r="K33" s="2" t="n"/>
+      <c r="L33" s="2" t="n"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="2" t="n"/>
+      <c r="B34" s="2" t="n"/>
+      <c r="C34" s="2" t="n"/>
+      <c r="D34" s="2" t="n"/>
+      <c r="E34" s="2" t="n"/>
+      <c r="F34" s="2" t="n"/>
+      <c r="G34" s="2" t="n"/>
+      <c r="H34" s="2" t="n"/>
+      <c r="I34" s="2" t="n"/>
+      <c r="J34" s="2" t="n"/>
+      <c r="K34" s="2" t="n"/>
+      <c r="L34" s="2" t="n"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="2" t="n"/>
+      <c r="B35" s="2" t="n"/>
+      <c r="C35" s="2" t="n"/>
+      <c r="D35" s="2" t="n"/>
+      <c r="E35" s="2" t="n"/>
+      <c r="F35" s="2" t="n"/>
+      <c r="G35" s="2" t="n"/>
+      <c r="H35" s="2" t="n"/>
+      <c r="I35" s="2" t="n"/>
+      <c r="J35" s="2" t="n"/>
+      <c r="K35" s="2" t="n"/>
+      <c r="L35" s="2" t="n"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="2" t="n"/>
+      <c r="B36" s="2" t="n"/>
+      <c r="C36" s="2" t="n"/>
+      <c r="D36" s="2" t="n"/>
+      <c r="E36" s="2" t="n"/>
+      <c r="F36" s="2" t="n"/>
+      <c r="G36" s="2" t="n"/>
+      <c r="H36" s="2" t="n"/>
+      <c r="I36" s="2" t="n"/>
+      <c r="J36" s="2" t="n"/>
+      <c r="K36" s="2" t="n"/>
+      <c r="L36" s="2" t="n"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="2" t="n"/>
+      <c r="B37" s="2" t="n"/>
+      <c r="C37" s="2" t="n"/>
+      <c r="D37" s="2" t="n"/>
+      <c r="E37" s="2" t="n"/>
+      <c r="F37" s="2" t="n"/>
+      <c r="G37" s="2" t="n"/>
+      <c r="H37" s="2" t="n"/>
+      <c r="I37" s="2" t="n"/>
+      <c r="J37" s="2" t="n"/>
+      <c r="K37" s="2" t="n"/>
+      <c r="L37" s="2" t="n"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="2" t="n"/>
+      <c r="B38" s="2" t="n"/>
+      <c r="C38" s="2" t="n"/>
+      <c r="D38" s="2" t="n"/>
+      <c r="E38" s="2" t="n"/>
+      <c r="F38" s="2" t="n"/>
+      <c r="G38" s="2" t="n"/>
+      <c r="H38" s="2" t="n"/>
+      <c r="I38" s="2" t="n"/>
+      <c r="J38" s="2" t="n"/>
+      <c r="K38" s="2" t="n"/>
+      <c r="L38" s="2" t="n"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="2" t="n"/>
+      <c r="B39" s="2" t="n"/>
+      <c r="C39" s="2" t="n"/>
+      <c r="D39" s="2" t="n"/>
+      <c r="E39" s="2" t="n"/>
+      <c r="F39" s="2" t="n"/>
+      <c r="G39" s="2" t="n"/>
+      <c r="H39" s="2" t="n"/>
+      <c r="I39" s="2" t="n"/>
+      <c r="J39" s="2" t="n"/>
+      <c r="K39" s="2" t="n"/>
+      <c r="L39" s="2" t="n"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="2" t="n"/>
+      <c r="B40" s="2" t="n"/>
+      <c r="C40" s="2" t="n"/>
+      <c r="D40" s="2" t="n"/>
+      <c r="E40" s="2" t="n"/>
+      <c r="F40" s="2" t="n"/>
+      <c r="G40" s="2" t="n"/>
+      <c r="H40" s="2" t="n"/>
+      <c r="I40" s="2" t="n"/>
+      <c r="J40" s="2" t="n"/>
+      <c r="K40" s="2" t="n"/>
+      <c r="L40" s="2" t="n"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="2" t="n"/>
+      <c r="B41" s="2" t="n"/>
+      <c r="C41" s="2" t="n"/>
+      <c r="D41" s="2" t="n"/>
+      <c r="E41" s="2" t="n"/>
+      <c r="F41" s="2" t="n"/>
+      <c r="G41" s="2" t="n"/>
+      <c r="H41" s="2" t="n"/>
+      <c r="I41" s="2" t="n"/>
+      <c r="J41" s="2" t="n"/>
+      <c r="K41" s="2" t="n"/>
+      <c r="L41" s="2" t="n"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="2" t="n"/>
+      <c r="B42" s="2" t="n"/>
+      <c r="C42" s="2" t="n"/>
+      <c r="D42" s="2" t="n"/>
+      <c r="E42" s="2" t="n"/>
+      <c r="F42" s="2" t="n"/>
+      <c r="G42" s="2" t="n"/>
+      <c r="H42" s="2" t="n"/>
+      <c r="I42" s="2" t="n"/>
+      <c r="J42" s="2" t="n"/>
+      <c r="K42" s="2" t="n"/>
+      <c r="L42" s="2" t="n"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="2" t="n"/>
+      <c r="B43" s="2" t="n"/>
+      <c r="C43" s="2" t="n"/>
+      <c r="D43" s="2" t="n"/>
+      <c r="E43" s="2" t="n"/>
+      <c r="F43" s="2" t="n"/>
+      <c r="G43" s="2" t="n"/>
+      <c r="H43" s="2" t="n"/>
+      <c r="I43" s="2" t="n"/>
+      <c r="J43" s="2" t="n"/>
+      <c r="K43" s="2" t="n"/>
+      <c r="L43" s="2" t="n"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="2" t="n"/>
+      <c r="B44" s="2" t="n"/>
+      <c r="C44" s="2" t="n"/>
+      <c r="D44" s="2" t="n"/>
+      <c r="E44" s="2" t="n"/>
+      <c r="F44" s="2" t="n"/>
+      <c r="G44" s="2" t="n"/>
+      <c r="H44" s="2" t="n"/>
+      <c r="I44" s="2" t="n"/>
+      <c r="J44" s="2" t="n"/>
+      <c r="K44" s="2" t="n"/>
+      <c r="L44" s="2" t="n"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="2" t="n"/>
+      <c r="B45" s="2" t="n"/>
+      <c r="C45" s="2" t="n"/>
+      <c r="D45" s="2" t="n"/>
+      <c r="E45" s="2" t="n"/>
+      <c r="F45" s="2" t="n"/>
+      <c r="G45" s="2" t="n"/>
+      <c r="H45" s="2" t="n"/>
+      <c r="I45" s="2" t="n"/>
+      <c r="J45" s="2" t="n"/>
+      <c r="K45" s="2" t="n"/>
+      <c r="L45" s="2" t="n"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="2" t="n"/>
+      <c r="B46" s="2" t="n"/>
+      <c r="C46" s="2" t="n"/>
+      <c r="D46" s="2" t="n"/>
+      <c r="E46" s="2" t="n"/>
+      <c r="F46" s="2" t="n"/>
+      <c r="G46" s="2" t="n"/>
+      <c r="H46" s="2" t="n"/>
+      <c r="I46" s="2" t="n"/>
+      <c r="J46" s="2" t="n"/>
+      <c r="K46" s="2" t="n"/>
+      <c r="L46" s="2" t="n"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="2" t="n"/>
+      <c r="B47" s="2" t="n"/>
+      <c r="C47" s="2" t="n"/>
+      <c r="D47" s="2" t="n"/>
+      <c r="E47" s="2" t="n"/>
+      <c r="F47" s="2" t="n"/>
+      <c r="G47" s="2" t="n"/>
+      <c r="H47" s="2" t="n"/>
+      <c r="I47" s="2" t="n"/>
+      <c r="J47" s="2" t="n"/>
+      <c r="K47" s="2" t="n"/>
+      <c r="L47" s="2" t="n"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="2" t="n"/>
+      <c r="B48" s="2" t="n"/>
+      <c r="C48" s="2" t="n"/>
+      <c r="D48" s="2" t="n"/>
+      <c r="E48" s="2" t="n"/>
+      <c r="F48" s="2" t="n"/>
+      <c r="G48" s="2" t="n"/>
+      <c r="H48" s="2" t="n"/>
+      <c r="I48" s="2" t="n"/>
+      <c r="J48" s="2" t="n"/>
+      <c r="K48" s="2" t="n"/>
+      <c r="L48" s="2" t="n"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="2" t="n"/>
+      <c r="B49" s="2" t="n"/>
+      <c r="C49" s="2" t="n"/>
+      <c r="D49" s="2" t="n"/>
+      <c r="E49" s="2" t="n"/>
+      <c r="F49" s="2" t="n"/>
+      <c r="G49" s="2" t="n"/>
+      <c r="H49" s="2" t="n"/>
+      <c r="I49" s="2" t="n"/>
+      <c r="J49" s="2" t="n"/>
+      <c r="K49" s="2" t="n"/>
+      <c r="L49" s="2" t="n"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="2" t="n"/>
+      <c r="B50" s="2" t="n"/>
+      <c r="C50" s="2" t="n"/>
+      <c r="D50" s="2" t="n"/>
+      <c r="E50" s="2" t="n"/>
+      <c r="F50" s="2" t="n"/>
+      <c r="G50" s="2" t="n"/>
+      <c r="H50" s="2" t="n"/>
+      <c r="I50" s="2" t="n"/>
+      <c r="J50" s="2" t="n"/>
+      <c r="K50" s="2" t="n"/>
+      <c r="L50" s="2" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I7:J7"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>